<commit_message>
add headers for sorting
</commit_message>
<xml_diff>
--- a/xlsxtra_test.xlsx
+++ b/xlsxtra_test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>hello</t>
   </si>
@@ -41,7 +41,7 @@
     <t>gender</t>
   </si>
   <si>
-    <t>ip_address</t>
+    <t>amount</t>
   </si>
   <si>
     <t>Jimmy</t>
@@ -56,9 +56,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>16.17.167.238</t>
-  </si>
-  <si>
     <t>Harry</t>
   </si>
   <si>
@@ -68,18 +65,12 @@
     <t>hhunter1@webnode.com</t>
   </si>
   <si>
-    <t>240.42.189.119</t>
-  </si>
-  <si>
     <t>Benjamin</t>
   </si>
   <si>
     <t>bmorgan2@unblog.fr</t>
   </si>
   <si>
-    <t>96.41.142.121</t>
-  </si>
-  <si>
     <t>Teresa</t>
   </si>
   <si>
@@ -89,27 +80,18 @@
     <t>Female</t>
   </si>
   <si>
-    <t>94.78.214.245</t>
-  </si>
-  <si>
     <t>Joshua</t>
   </si>
   <si>
     <t>jstone4@google.cn</t>
   </si>
   <si>
-    <t>125.32.19.210</t>
-  </si>
-  <si>
     <t>Rose</t>
   </si>
   <si>
     <t>rjohnson5@odnoklassniki.ru</t>
   </si>
   <si>
-    <t>29.139.205.214</t>
-  </si>
-  <si>
     <t>Donald</t>
   </si>
   <si>
@@ -119,36 +101,28 @@
     <t>dbryant6@redcross.org</t>
   </si>
   <si>
-    <t>57.28.4.238</t>
-  </si>
-  <si>
     <t>Jacqueline</t>
   </si>
   <si>
     <t>jfields7@dagondesign.com</t>
   </si>
   <si>
-    <t>165.182.190.97</t>
-  </si>
-  <si>
     <t>lharper8@wunderground.com</t>
   </si>
   <si>
-    <t>171.36.193.204</t>
-  </si>
-  <si>
     <t>hmarshall9@stumbleupon.com</t>
   </si>
   <si>
-    <t>74.236.54.34</t>
+    <t>€ 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="[$€-413]\ #,##0.00;[RED][$€-413]\ #,##0.00\-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -215,8 +189,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,7 +218,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B10 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -272,7 +250,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -322,8 +300,8 @@
       <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>11</v>
+      <c r="F2" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,19 +309,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>15</v>
+      <c r="F3" s="0" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,19 +329,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>18</v>
+      <c r="F4" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,19 +349,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>6000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,19 +369,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>25</v>
+      <c r="F6" s="0" t="n">
+        <v>50000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,19 +389,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>400000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,19 +409,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>32</v>
+      <c r="F8" s="0" t="n">
+        <v>3000000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,19 +429,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>20000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,19 +449,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>100000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,19 +469,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="E11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>